<commit_message>
averaged ptm plot in nb
</commit_message>
<xml_diff>
--- a/analyses/T7-incubations/unipept/GO/organizing/BY_GO.xlsx
+++ b/analyses/T7-incubations/unipept/GO/organizing/BY_GO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="978">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1681" uniqueCount="978">
   <si>
     <t xml:space="preserve">102_BY_T00_GF</t>
   </si>
@@ -3059,7 +3059,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="1" sqref="G1:K10 E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3671,7 +3671,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="1" sqref="G1:K10 F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3983,7 +3983,7 @@
   <dimension ref="A1:L296"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="G1:K10 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11354,10 +11354,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11378,10 +11378,25 @@
       <c r="E1" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>67</v>
@@ -11395,10 +11410,29 @@
       <c r="E2" s="0" t="n">
         <v>31</v>
       </c>
+      <c r="G2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <f aca="false">B2/B$11*100</f>
+        <v>32.3671497584541</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <f aca="false">C2/C$11*100</f>
+        <v>26.8518518518519</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <f aca="false">D2/D$11*100</f>
+        <v>26.3005780346821</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <f aca="false">E2/E$11*100</f>
+        <v>27.4336283185841</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>42</v>
@@ -11412,10 +11446,29 @@
       <c r="E3" s="0" t="n">
         <v>29</v>
       </c>
+      <c r="G3" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">B3/B$11*100</f>
+        <v>20.2898550724638</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <f aca="false">C3/C$11*100</f>
+        <v>23.1481481481481</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <f aca="false">D3/D$11*100</f>
+        <v>22.2543352601156</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <f aca="false">E3/E$11*100</f>
+        <v>25.6637168141593</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>41</v>
@@ -11429,10 +11482,29 @@
       <c r="E4" s="0" t="n">
         <v>24</v>
       </c>
+      <c r="G4" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">B4/B$11*100</f>
+        <v>19.8067632850242</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <f aca="false">C4/C$11*100</f>
+        <v>15.7407407407407</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <f aca="false">D4/D$11*100</f>
+        <v>21.9653179190751</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <f aca="false">E4/E$11*100</f>
+        <v>21.2389380530973</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>12</v>
@@ -11446,10 +11518,29 @@
       <c r="E5" s="0" t="n">
         <v>9</v>
       </c>
+      <c r="G5" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">B5/B$11*100</f>
+        <v>5.79710144927536</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <f aca="false">C5/C$11*100</f>
+        <v>6.48148148148148</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <f aca="false">D5/D$11*100</f>
+        <v>4.04624277456647</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <f aca="false">E5/E$11*100</f>
+        <v>7.9646017699115</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>12</v>
@@ -11463,10 +11554,29 @@
       <c r="E6" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="G6" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <f aca="false">B6/B$11*100</f>
+        <v>5.79710144927536</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <f aca="false">C6/C$11*100</f>
+        <v>7.40740740740741</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <f aca="false">D6/D$11*100</f>
+        <v>4.91329479768786</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <f aca="false">E6/E$11*100</f>
+        <v>5.30973451327434</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>11</v>
@@ -11480,10 +11590,29 @@
       <c r="E7" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="G7" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <f aca="false">B7/B$11*100</f>
+        <v>5.31400966183575</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <f aca="false">C7/C$11*100</f>
+        <v>4.62962962962963</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <f aca="false">D7/D$11*100</f>
+        <v>6.06936416184971</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <f aca="false">E7/E$11*100</f>
+        <v>2.65486725663717</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>10</v>
@@ -11497,10 +11626,29 @@
       <c r="E8" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="G8" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <f aca="false">B8/B$11*100</f>
+        <v>4.83091787439614</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <f aca="false">C8/C$11*100</f>
+        <v>6.48148148148148</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <f aca="false">D8/D$11*100</f>
+        <v>5.78034682080925</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <f aca="false">E8/E$11*100</f>
+        <v>2.65486725663717</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>8</v>
@@ -11514,10 +11662,29 @@
       <c r="E9" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G9" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <f aca="false">B9/B$11*100</f>
+        <v>3.86473429951691</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <f aca="false">C9/C$11*100</f>
+        <v>4.62962962962963</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <f aca="false">D9/D$11*100</f>
+        <v>5.78034682080925</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <f aca="false">E9/E$11*100</f>
+        <v>3.53982300884956</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>4</v>
@@ -11530,6 +11697,46 @@
       </c>
       <c r="E10" s="0" t="n">
         <v>4</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <f aca="false">B10/B$11*100</f>
+        <v>1.93236714975845</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <f aca="false">C10/C$11*100</f>
+        <v>4.62962962962963</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <f aca="false">D10/D$11*100</f>
+        <v>2.89017341040462</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <f aca="false">E10/E$11*100</f>
+        <v>3.53982300884956</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <f aca="false">SUM(B2:B10)</f>
+        <v>207</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <f aca="false">SUM(C2:C10)</f>
+        <v>108</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <f aca="false">SUM(D2:D10)</f>
+        <v>346</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <f aca="false">SUM(E2:E10)</f>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
plotted all four t7 mf go heatmaps
</commit_message>
<xml_diff>
--- a/analyses/T7-incubations/unipept/GO/organizing/BY_GO.xlsx
+++ b/analyses/T7-incubations/unipept/GO/organizing/BY_GO.xlsx
@@ -2963,8 +2963,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -3031,12 +3032,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3063,7 +3068,7 @@
       <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3656,7 +3661,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3675,7 +3680,7 @@
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3968,7 +3973,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3987,7 +3992,7 @@
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.71"/>
@@ -3995,7 +4000,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="33.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="30.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="30.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="43.19"/>
@@ -4426,14 +4431,14 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="2" t="n">
         <f aca="false">SUM(A33:A34)</f>
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D12" s="1" t="n">
@@ -4535,7 +4540,7 @@
       <c r="I14" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J14" s="0" t="n">
+      <c r="J14" s="2" t="n">
         <f aca="false">SUM(J20:J28)</f>
         <v>10</v>
       </c>
@@ -4594,7 +4599,7 @@
       <c r="C16" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -4603,7 +4608,7 @@
       <c r="F16" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="2" t="n">
         <v>0</v>
       </c>
       <c r="H16" s="1" t="s">
@@ -4612,7 +4617,7 @@
       <c r="I16" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J16" s="0" t="n">
+      <c r="J16" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K16" s="1" t="s">
@@ -4630,7 +4635,7 @@
       <c r="C17" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="2" t="n">
         <f aca="false">SUM(D50:D56)</f>
         <v>23</v>
       </c>
@@ -4638,18 +4643,18 @@
       <c r="F17" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="2" t="n">
         <f aca="false">SUM(G50:G56)</f>
         <v>44</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="J17" s="0" t="n">
+      <c r="J17" s="2" t="n">
         <f aca="false">SUM(J50:J56)</f>
         <v>22</v>
       </c>
-      <c r="K17" s="0"/>
+      <c r="K17" s="2"/>
       <c r="L17" s="1" t="s">
         <v>94</v>
       </c>
@@ -4682,9 +4687,9 @@
       <c r="I19" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J19" s="0"/>
-      <c r="K19" s="0"/>
-      <c r="L19" s="0"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -4734,7 +4739,7 @@
       <c r="C21" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F21" s="0"/>
+      <c r="F21" s="2"/>
       <c r="G21" s="1" t="n">
         <v>4</v>
       </c>
@@ -5114,7 +5119,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F36" s="0"/>
+      <c r="F36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
@@ -5346,9 +5351,9 @@
       <c r="I45" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J45" s="0"/>
-      <c r="K45" s="0"/>
-      <c r="L45" s="0"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D46" s="1"/>
@@ -5406,12 +5411,12 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G49" s="0"/>
-      <c r="H49" s="0"/>
-      <c r="I49" s="0"/>
-      <c r="J49" s="0"/>
-      <c r="K49" s="0"/>
-      <c r="L49" s="0"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
@@ -9434,9 +9439,9 @@
       <c r="I155" s="1" t="s">
         <v>702</v>
       </c>
-      <c r="J155" s="0"/>
-      <c r="K155" s="0"/>
-      <c r="L155" s="0"/>
+      <c r="J155" s="2"/>
+      <c r="K155" s="2"/>
+      <c r="L155" s="2"/>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="n">
@@ -9719,9 +9724,9 @@
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="0"/>
-      <c r="B170" s="0"/>
-      <c r="C170" s="0"/>
+      <c r="A170" s="2"/>
+      <c r="B170" s="2"/>
+      <c r="C170" s="2"/>
       <c r="G170" s="1" t="n">
         <v>1</v>
       </c>
@@ -11488,14 +11493,14 @@
       </c>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G306" s="0"/>
-      <c r="H306" s="0"/>
-      <c r="I306" s="0"/>
+      <c r="G306" s="2"/>
+      <c r="H306" s="2"/>
+      <c r="I306" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -11510,11 +11515,11 @@
   </sheetPr>
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N26" activeCellId="0" sqref="N26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M22" activeCellId="0" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -11916,7 +11921,7 @@
       <c r="E14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="2" t="s">
         <v>977</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -11942,25 +11947,25 @@
       <c r="C15" s="1" t="n">
         <v>91</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="2" t="n">
         <v>31</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="2" t="n">
         <f aca="false">(B15/B$31)*100</f>
         <v>21.6828478964401</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15" s="2" t="n">
         <f aca="false">(C15/C$31)*100</f>
         <v>19.2389006342495</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="I15" s="2" t="n">
         <f aca="false">(D15/D$31)*100</f>
         <v>18.125</v>
       </c>
-      <c r="J15" s="0" t="n">
+      <c r="J15" s="2" t="n">
         <f aca="false">(E15/E$31)*100</f>
         <v>19.2546583850932</v>
       </c>
@@ -11975,25 +11980,25 @@
       <c r="C16" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="2" t="n">
         <f aca="false">(B16/B$31)*100</f>
         <v>3.88349514563107</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16" s="2" t="n">
         <f aca="false">(C16/C$31)*100</f>
         <v>3.59408033826638</v>
       </c>
-      <c r="I16" s="0" t="n">
+      <c r="I16" s="2" t="n">
         <f aca="false">(D16/D$31)*100</f>
         <v>5</v>
       </c>
-      <c r="J16" s="0" t="n">
+      <c r="J16" s="2" t="n">
         <f aca="false">(E16/E$31)*100</f>
         <v>3.72670807453416</v>
       </c>
@@ -12008,25 +12013,25 @@
       <c r="C17" s="1" t="n">
         <v>108</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="2" t="n">
         <f aca="false">(B17/B$31)*100</f>
         <v>19.0938511326861</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="H17" s="2" t="n">
         <f aca="false">(C17/C$31)*100</f>
         <v>22.8329809725159</v>
       </c>
-      <c r="I17" s="0" t="n">
+      <c r="I17" s="2" t="n">
         <f aca="false">(D17/D$31)*100</f>
         <v>20</v>
       </c>
-      <c r="J17" s="0" t="n">
+      <c r="J17" s="2" t="n">
         <f aca="false">(E17/E$31)*100</f>
         <v>18.0124223602484</v>
       </c>
@@ -12041,25 +12046,25 @@
       <c r="C18" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="2" t="n">
         <f aca="false">(B18/B$31)*100</f>
         <v>5.17799352750809</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H18" s="2" t="n">
         <f aca="false">(C18/C$31)*100</f>
         <v>4.22832980972516</v>
       </c>
-      <c r="I18" s="0" t="n">
+      <c r="I18" s="2" t="n">
         <f aca="false">(D18/D$31)*100</f>
         <v>7.5</v>
       </c>
-      <c r="J18" s="0" t="n">
+      <c r="J18" s="2" t="n">
         <f aca="false">(E18/E$31)*100</f>
         <v>1.86335403726708</v>
       </c>
@@ -12074,25 +12079,25 @@
       <c r="C19" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="D19" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E19" s="0" t="n">
+      <c r="D19" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="2" t="n">
         <f aca="false">(B19/B$31)*100</f>
         <v>1.29449838187702</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="H19" s="2" t="n">
         <f aca="false">(C19/C$31)*100</f>
         <v>1.90274841437632</v>
       </c>
-      <c r="I19" s="0" t="n">
+      <c r="I19" s="2" t="n">
         <f aca="false">(D19/D$31)*100</f>
         <v>1.25</v>
       </c>
-      <c r="J19" s="0" t="n">
+      <c r="J19" s="2" t="n">
         <f aca="false">(E19/E$31)*100</f>
         <v>1.86335403726708</v>
       </c>
@@ -12107,25 +12112,25 @@
       <c r="C20" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="G20" s="2" t="n">
         <f aca="false">(B20/B$31)*100</f>
         <v>4.53074433656958</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="H20" s="2" t="n">
         <f aca="false">(C20/C$31)*100</f>
         <v>4.22832980972516</v>
       </c>
-      <c r="I20" s="0" t="n">
+      <c r="I20" s="2" t="n">
         <f aca="false">(D20/D$31)*100</f>
         <v>3.125</v>
       </c>
-      <c r="J20" s="0" t="n">
+      <c r="J20" s="2" t="n">
         <f aca="false">(E20/E$31)*100</f>
         <v>2.48447204968944</v>
       </c>
@@ -12140,25 +12145,25 @@
       <c r="C21" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="G21" s="0" t="n">
+      <c r="G21" s="2" t="n">
         <f aca="false">(B21/B$31)*100</f>
         <v>3.88349514563107</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="H21" s="2" t="n">
         <f aca="false">(C21/C$31)*100</f>
         <v>2.95983086680761</v>
       </c>
-      <c r="I21" s="0" t="n">
+      <c r="I21" s="2" t="n">
         <f aca="false">(D21/D$31)*100</f>
         <v>4.375</v>
       </c>
-      <c r="J21" s="0" t="n">
+      <c r="J21" s="2" t="n">
         <f aca="false">(E21/E$31)*100</f>
         <v>5.59006211180124</v>
       </c>
@@ -12173,25 +12178,25 @@
       <c r="C22" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="G22" s="0" t="n">
+      <c r="G22" s="2" t="n">
         <f aca="false">(B22/B$31)*100</f>
         <v>13.2686084142395</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="H22" s="2" t="n">
         <f aca="false">(C22/C$31)*100</f>
         <v>16.0676532769556</v>
       </c>
-      <c r="I22" s="0" t="n">
+      <c r="I22" s="2" t="n">
         <f aca="false">(D22/D$31)*100</f>
         <v>10.625</v>
       </c>
-      <c r="J22" s="0" t="n">
+      <c r="J22" s="2" t="n">
         <f aca="false">(E22/E$31)*100</f>
         <v>14.9068322981366</v>
       </c>
@@ -12206,25 +12211,25 @@
       <c r="C23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="G23" s="0" t="n">
+      <c r="G23" s="2" t="n">
         <f aca="false">(B23/B$31)*100</f>
         <v>3.55987055016181</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="H23" s="2" t="n">
         <f aca="false">(C23/C$31)*100</f>
         <v>4.43974630021142</v>
       </c>
-      <c r="I23" s="0" t="n">
+      <c r="I23" s="2" t="n">
         <f aca="false">(D23/D$31)*100</f>
         <v>3.125</v>
       </c>
-      <c r="J23" s="0" t="n">
+      <c r="J23" s="2" t="n">
         <f aca="false">(E23/E$31)*100</f>
         <v>1.86335403726708</v>
       </c>
@@ -12239,25 +12244,25 @@
       <c r="C24" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="G24" s="2" t="n">
         <f aca="false">(B24/B$31)*100</f>
         <v>1.29449838187702</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="H24" s="2" t="n">
         <f aca="false">(C24/C$31)*100</f>
         <v>0.211416490486258</v>
       </c>
-      <c r="I24" s="0" t="n">
+      <c r="I24" s="2" t="n">
         <f aca="false">(D24/D$31)*100</f>
         <v>1.875</v>
       </c>
-      <c r="J24" s="0" t="n">
+      <c r="J24" s="2" t="n">
         <f aca="false">(E24/E$31)*100</f>
         <v>2.48447204968944</v>
       </c>
@@ -12272,25 +12277,25 @@
       <c r="C25" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="D25" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G25" s="0" t="n">
+      <c r="D25" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" s="2" t="n">
         <f aca="false">(B25/B$31)*100</f>
         <v>1.94174757281553</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="H25" s="2" t="n">
         <f aca="false">(C25/C$31)*100</f>
         <v>2.53699788583509</v>
       </c>
-      <c r="I25" s="0" t="n">
+      <c r="I25" s="2" t="n">
         <f aca="false">(D25/D$31)*100</f>
         <v>1.25</v>
       </c>
-      <c r="J25" s="0" t="n">
+      <c r="J25" s="2" t="n">
         <f aca="false">(E25/E$31)*100</f>
         <v>0.62111801242236</v>
       </c>
@@ -12305,25 +12310,25 @@
       <c r="C26" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="G26" s="2" t="n">
         <f aca="false">(B26/B$31)*100</f>
         <v>2.26537216828479</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="H26" s="2" t="n">
         <f aca="false">(C26/C$31)*100</f>
         <v>2.11416490486258</v>
       </c>
-      <c r="I26" s="0" t="n">
+      <c r="I26" s="2" t="n">
         <f aca="false">(D26/D$31)*100</f>
         <v>3.125</v>
       </c>
-      <c r="J26" s="0" t="n">
+      <c r="J26" s="2" t="n">
         <f aca="false">(E26/E$31)*100</f>
         <v>2.48447204968944</v>
       </c>
@@ -12338,25 +12343,25 @@
       <c r="C27" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="G27" s="0" t="n">
+      <c r="G27" s="2" t="n">
         <f aca="false">(B27/B$31)*100</f>
         <v>6.79611650485437</v>
       </c>
-      <c r="H27" s="0" t="n">
+      <c r="H27" s="2" t="n">
         <f aca="false">(C27/C$31)*100</f>
         <v>6.34249471458774</v>
       </c>
-      <c r="I27" s="0" t="n">
+      <c r="I27" s="2" t="n">
         <f aca="false">(D27/D$31)*100</f>
         <v>5</v>
       </c>
-      <c r="J27" s="0" t="n">
+      <c r="J27" s="2" t="n">
         <f aca="false">(E27/E$31)*100</f>
         <v>6.2111801242236</v>
       </c>
@@ -12371,25 +12376,25 @@
       <c r="C28" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D28" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E28" s="0" t="n">
+      <c r="D28" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E28" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="G28" s="0" t="n">
+      <c r="G28" s="2" t="n">
         <f aca="false">(B28/B$31)*100</f>
         <v>1.61812297734628</v>
       </c>
-      <c r="H28" s="0" t="n">
+      <c r="H28" s="2" t="n">
         <f aca="false">(C28/C$31)*100</f>
         <v>0</v>
       </c>
-      <c r="I28" s="0" t="n">
+      <c r="I28" s="2" t="n">
         <f aca="false">(D28/D$31)*100</f>
         <v>1.25</v>
       </c>
-      <c r="J28" s="0" t="n">
+      <c r="J28" s="2" t="n">
         <f aca="false">(E28/E$31)*100</f>
         <v>4.96894409937888</v>
       </c>
@@ -12404,25 +12409,25 @@
       <c r="C29" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="E29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G29" s="0" t="n">
+      <c r="G29" s="2" t="n">
         <f aca="false">(B29/B$31)*100</f>
         <v>0</v>
       </c>
-      <c r="H29" s="0" t="n">
+      <c r="H29" s="2" t="n">
         <f aca="false">(C29/C$31)*100</f>
         <v>0</v>
       </c>
-      <c r="I29" s="0" t="n">
+      <c r="I29" s="2" t="n">
         <f aca="false">(D29/D$31)*100</f>
         <v>0</v>
       </c>
-      <c r="J29" s="0" t="n">
+      <c r="J29" s="2" t="n">
         <f aca="false">(E29/E$31)*100</f>
         <v>0</v>
       </c>
@@ -12437,62 +12442,62 @@
       <c r="C30" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="G30" s="0" t="n">
+      <c r="G30" s="2" t="n">
         <f aca="false">(B30/B$31)*100</f>
         <v>9.70873786407767</v>
       </c>
-      <c r="H30" s="0" t="n">
+      <c r="H30" s="2" t="n">
         <f aca="false">(C30/C$31)*100</f>
         <v>9.30232558139535</v>
       </c>
-      <c r="I30" s="0" t="n">
+      <c r="I30" s="2" t="n">
         <f aca="false">(D30/D$31)*100</f>
         <v>14.375</v>
       </c>
-      <c r="J30" s="0" t="n">
+      <c r="J30" s="2" t="n">
         <f aca="false">(E30/E$31)*100</f>
         <v>13.6645962732919</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="2" t="n">
         <f aca="false">SUM(B15:B30)</f>
         <v>309</v>
       </c>
-      <c r="C31" s="0" t="n">
+      <c r="C31" s="2" t="n">
         <f aca="false">SUM(C15:C30)</f>
         <v>473</v>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="D31" s="2" t="n">
         <f aca="false">SUM(D15:D30)</f>
         <v>160</v>
       </c>
-      <c r="E31" s="0" t="n">
+      <c r="E31" s="2" t="n">
         <f aca="false">SUM(E15:E30)</f>
         <v>161</v>
       </c>
-      <c r="G31" s="0" t="n">
+      <c r="G31" s="2" t="n">
         <f aca="false">(B31/B$31)*100</f>
         <v>100</v>
       </c>
-      <c r="H31" s="0" t="n">
+      <c r="H31" s="2" t="n">
         <f aca="false">(C31/C$31)*100</f>
         <v>100</v>
       </c>
-      <c r="I31" s="0" t="n">
+      <c r="I31" s="2" t="n">
         <f aca="false">(D31/D$31)*100</f>
         <v>100</v>
       </c>
-      <c r="J31" s="0" t="n">
+      <c r="J31" s="2" t="n">
         <f aca="false">(E31/E$31)*100</f>
         <v>100</v>
       </c>
@@ -12500,7 +12505,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
workaround for cbar label still not great
</commit_message>
<xml_diff>
--- a/analyses/T7-incubations/unipept/GO/organizing/BY_GO.xlsx
+++ b/analyses/T7-incubations/unipept/GO/organizing/BY_GO.xlsx
@@ -2963,9 +2963,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -3032,7 +3033,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3042,6 +3043,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3068,7 +3073,7 @@
       <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3680,7 +3685,7 @@
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3992,7 +3997,7 @@
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.71"/>
@@ -11516,10 +11521,10 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M22" activeCellId="0" sqref="M22"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -11961,7 +11966,7 @@
         <f aca="false">(C15/C$31)*100</f>
         <v>19.2389006342495</v>
       </c>
-      <c r="I15" s="2" t="n">
+      <c r="I15" s="3" t="n">
         <f aca="false">(D15/D$31)*100</f>
         <v>18.125</v>
       </c>
@@ -11994,7 +11999,7 @@
         <f aca="false">(C16/C$31)*100</f>
         <v>3.59408033826638</v>
       </c>
-      <c r="I16" s="2" t="n">
+      <c r="I16" s="3" t="n">
         <f aca="false">(D16/D$31)*100</f>
         <v>5</v>
       </c>
@@ -12027,7 +12032,7 @@
         <f aca="false">(C17/C$31)*100</f>
         <v>22.8329809725159</v>
       </c>
-      <c r="I17" s="2" t="n">
+      <c r="I17" s="3" t="n">
         <f aca="false">(D17/D$31)*100</f>
         <v>20</v>
       </c>
@@ -12060,7 +12065,7 @@
         <f aca="false">(C18/C$31)*100</f>
         <v>4.22832980972516</v>
       </c>
-      <c r="I18" s="2" t="n">
+      <c r="I18" s="3" t="n">
         <f aca="false">(D18/D$31)*100</f>
         <v>7.5</v>
       </c>
@@ -12093,7 +12098,7 @@
         <f aca="false">(C19/C$31)*100</f>
         <v>1.90274841437632</v>
       </c>
-      <c r="I19" s="2" t="n">
+      <c r="I19" s="3" t="n">
         <f aca="false">(D19/D$31)*100</f>
         <v>1.25</v>
       </c>
@@ -12126,7 +12131,7 @@
         <f aca="false">(C20/C$31)*100</f>
         <v>4.22832980972516</v>
       </c>
-      <c r="I20" s="2" t="n">
+      <c r="I20" s="3" t="n">
         <f aca="false">(D20/D$31)*100</f>
         <v>3.125</v>
       </c>
@@ -12159,7 +12164,7 @@
         <f aca="false">(C21/C$31)*100</f>
         <v>2.95983086680761</v>
       </c>
-      <c r="I21" s="2" t="n">
+      <c r="I21" s="3" t="n">
         <f aca="false">(D21/D$31)*100</f>
         <v>4.375</v>
       </c>
@@ -12192,7 +12197,7 @@
         <f aca="false">(C22/C$31)*100</f>
         <v>16.0676532769556</v>
       </c>
-      <c r="I22" s="2" t="n">
+      <c r="I22" s="3" t="n">
         <f aca="false">(D22/D$31)*100</f>
         <v>10.625</v>
       </c>
@@ -12225,7 +12230,7 @@
         <f aca="false">(C23/C$31)*100</f>
         <v>4.43974630021142</v>
       </c>
-      <c r="I23" s="2" t="n">
+      <c r="I23" s="3" t="n">
         <f aca="false">(D23/D$31)*100</f>
         <v>3.125</v>
       </c>
@@ -12258,7 +12263,7 @@
         <f aca="false">(C24/C$31)*100</f>
         <v>0.211416490486258</v>
       </c>
-      <c r="I24" s="2" t="n">
+      <c r="I24" s="3" t="n">
         <f aca="false">(D24/D$31)*100</f>
         <v>1.875</v>
       </c>
@@ -12291,7 +12296,7 @@
         <f aca="false">(C25/C$31)*100</f>
         <v>2.53699788583509</v>
       </c>
-      <c r="I25" s="2" t="n">
+      <c r="I25" s="3" t="n">
         <f aca="false">(D25/D$31)*100</f>
         <v>1.25</v>
       </c>
@@ -12324,7 +12329,7 @@
         <f aca="false">(C26/C$31)*100</f>
         <v>2.11416490486258</v>
       </c>
-      <c r="I26" s="2" t="n">
+      <c r="I26" s="3" t="n">
         <f aca="false">(D26/D$31)*100</f>
         <v>3.125</v>
       </c>
@@ -12357,7 +12362,7 @@
         <f aca="false">(C27/C$31)*100</f>
         <v>6.34249471458774</v>
       </c>
-      <c r="I27" s="2" t="n">
+      <c r="I27" s="3" t="n">
         <f aca="false">(D27/D$31)*100</f>
         <v>5</v>
       </c>
@@ -12390,7 +12395,7 @@
         <f aca="false">(C28/C$31)*100</f>
         <v>0</v>
       </c>
-      <c r="I28" s="2" t="n">
+      <c r="I28" s="3" t="n">
         <f aca="false">(D28/D$31)*100</f>
         <v>1.25</v>
       </c>
@@ -12423,7 +12428,7 @@
         <f aca="false">(C29/C$31)*100</f>
         <v>0</v>
       </c>
-      <c r="I29" s="2" t="n">
+      <c r="I29" s="3" t="n">
         <f aca="false">(D29/D$31)*100</f>
         <v>0</v>
       </c>
@@ -12456,7 +12461,7 @@
         <f aca="false">(C30/C$31)*100</f>
         <v>9.30232558139535</v>
       </c>
-      <c r="I30" s="2" t="n">
+      <c r="I30" s="3" t="n">
         <f aca="false">(D30/D$31)*100</f>
         <v>14.375</v>
       </c>

</xml_diff>